<commit_message>
Memperbarui ekspor excel untuk admin dan pengguna
</commit_message>
<xml_diff>
--- a/rekap_presensi.xlsx
+++ b/rekap_presensi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Tanggal</t>
   </si>
@@ -71,6 +71,15 @@
     <t>Jumat, 12 Mei 2023</t>
   </si>
   <si>
+    <t>09:43:26</t>
+  </si>
+  <si>
+    <t>Hadir</t>
+  </si>
+  <si>
+    <t>14,626 kilometer, TERLAMBAT 2 jam 29 menit</t>
+  </si>
+  <si>
     <t>Sabtu, 13 Mei 2023</t>
   </si>
   <si>
@@ -92,6 +101,15 @@
     <t>Jumat, 19 Mei 2023</t>
   </si>
   <si>
+    <t>21:01:29</t>
+  </si>
+  <si>
+    <t>22:22:48</t>
+  </si>
+  <si>
+    <t>34,163 kilometer, TERLAMBAT 13 jam 47 menit</t>
+  </si>
+  <si>
     <t>Sabtu, 20 Mei 2023</t>
   </si>
   <si>
@@ -105,15 +123,6 @@
   </si>
   <si>
     <t>Rabu, 24 Mei 2023</t>
-  </si>
-  <si>
-    <t>13:10:27</t>
-  </si>
-  <si>
-    <t>Hadir</t>
-  </si>
-  <si>
-    <t>13,535 kilometer</t>
   </si>
   <si>
     <t>Kamis, 25 Mei 2023</t>
@@ -529,7 +538,7 @@
     <col min="2" max="2" width="13" customWidth="true" style="0"/>
     <col min="3" max="3" width="13" customWidth="true" style="0"/>
     <col min="4" max="4" width="8" customWidth="true" style="0"/>
-    <col min="5" max="5" width="27" customWidth="true" style="0"/>
+    <col min="5" max="5" width="45" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -654,14 +663,20 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -670,7 +685,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -681,7 +696,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -690,7 +705,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -699,7 +714,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -708,7 +723,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -717,16 +732,24 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -735,7 +758,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -746,7 +769,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -755,7 +778,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -764,22 +787,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -788,7 +805,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -797,7 +814,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -806,7 +823,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -817,7 +834,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -826,7 +843,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -835,7 +852,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -844,15 +861,15 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -860,7 +877,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -868,10 +885,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memperbarui sistem CRUD Pengguna
</commit_message>
<xml_diff>
--- a/rekap_presensi.xlsx
+++ b/rekap_presensi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>Tanggal</t>
   </si>
@@ -71,43 +71,34 @@
     <t>Jumat, 12 Mei 2023</t>
   </si>
   <si>
-    <t>09:43:26</t>
+    <t>Sabtu, 13 Mei 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 14 Mei 2023</t>
+  </si>
+  <si>
+    <t>Senin, 15 Mei 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 16 Mei 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 17 Mei 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 18 Mei 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 19 Mei 2023</t>
+  </si>
+  <si>
+    <t>09:26:41</t>
   </si>
   <si>
     <t>Hadir</t>
   </si>
   <si>
-    <t>14,626 kilometer, TERLAMBAT 2 jam 29 menit</t>
-  </si>
-  <si>
-    <t>Sabtu, 13 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 14 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 15 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 16 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 17 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 18 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 19 Mei 2023</t>
-  </si>
-  <si>
-    <t>21:01:29</t>
-  </si>
-  <si>
-    <t>22:22:48</t>
-  </si>
-  <si>
-    <t>34,163 kilometer, TERLAMBAT 13 jam 47 menit</t>
+    <t>94,975 kilometer, TERLAMBAT 2 jam 12 menit</t>
   </si>
   <si>
     <t>Sabtu, 20 Mei 2023</t>
@@ -116,6 +107,15 @@
     <t>Minggu, 21 Mei 2023</t>
   </si>
   <si>
+    <t>21:42:21</t>
+  </si>
+  <si>
+    <t>21:42:54</t>
+  </si>
+  <si>
+    <t>34,744 kilometer, TERLAMBAT 14 jam 28 menit</t>
+  </si>
+  <si>
     <t>Senin, 22 Mei 2023</t>
   </si>
   <si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Rabu, 24 Mei 2023</t>
+  </si>
+  <si>
+    <t>17:42:33</t>
+  </si>
+  <si>
+    <t>14,626 kilometer, TERLAMBAT 10 jam 28 menit</t>
   </si>
   <si>
     <t>Kamis, 25 Mei 2023</t>
@@ -663,20 +669,14 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -685,7 +685,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -696,7 +696,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -705,7 +705,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -714,7 +714,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -723,7 +723,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -732,24 +732,22 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -758,13 +756,19 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -789,14 +793,20 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -805,7 +815,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -814,7 +824,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -823,7 +833,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -834,7 +844,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -843,7 +853,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -852,7 +862,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -861,15 +871,15 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -877,7 +887,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -885,10 +895,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B37" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Menambahkan fitur Rekap Absensi Harian
</commit_message>
<xml_diff>
--- a/rekap_presensi.xlsx
+++ b/rekap_presensi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Tanggal</t>
   </si>
@@ -71,6 +71,15 @@
     <t>Jumat, 12 Mei 2023</t>
   </si>
   <si>
+    <t>09:43:26</t>
+  </si>
+  <si>
+    <t>Hadir</t>
+  </si>
+  <si>
+    <t>14,626 kilometer, TERLAMBAT 2 jam 29 menit</t>
+  </si>
+  <si>
     <t>Sabtu, 13 Mei 2023</t>
   </si>
   <si>
@@ -92,13 +101,13 @@
     <t>Jumat, 19 Mei 2023</t>
   </si>
   <si>
-    <t>09:26:41</t>
-  </si>
-  <si>
-    <t>Hadir</t>
-  </si>
-  <si>
-    <t>94,975 kilometer, TERLAMBAT 2 jam 12 menit</t>
+    <t>21:01:29</t>
+  </si>
+  <si>
+    <t>22:22:48</t>
+  </si>
+  <si>
+    <t>34,163 kilometer, TERLAMBAT 13 jam 47 menit</t>
   </si>
   <si>
     <t>Sabtu, 20 Mei 2023</t>
@@ -107,15 +116,6 @@
     <t>Minggu, 21 Mei 2023</t>
   </si>
   <si>
-    <t>21:42:21</t>
-  </si>
-  <si>
-    <t>21:42:54</t>
-  </si>
-  <si>
-    <t>34,744 kilometer, TERLAMBAT 14 jam 28 menit</t>
-  </si>
-  <si>
     <t>Senin, 22 Mei 2023</t>
   </si>
   <si>
@@ -123,12 +123,6 @@
   </si>
   <si>
     <t>Rabu, 24 Mei 2023</t>
-  </si>
-  <si>
-    <t>17:42:33</t>
-  </si>
-  <si>
-    <t>14,626 kilometer, TERLAMBAT 10 jam 28 menit</t>
   </si>
   <si>
     <t>Kamis, 25 Mei 2023</t>
@@ -669,14 +663,20 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -685,7 +685,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -696,7 +696,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -705,7 +705,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -714,7 +714,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -723,7 +723,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -732,22 +732,24 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -756,19 +758,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -793,20 +789,14 @@
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -815,7 +805,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -824,7 +814,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -833,7 +823,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -844,7 +834,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -853,7 +843,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -862,7 +852,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -871,15 +861,15 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B34" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -887,7 +877,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -895,10 +885,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B37" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Memperbaiki halaman Beranda di dashboard admin
</commit_message>
<xml_diff>
--- a/rekap_presensi.xlsx
+++ b/rekap_presensi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Tanggal</t>
   </si>
@@ -71,79 +71,70 @@
     <t>Jumat, 12 Mei 2023</t>
   </si>
   <si>
-    <t>09:43:26</t>
+    <t>Sabtu, 13 Mei 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 14 Mei 2023</t>
+  </si>
+  <si>
+    <t>Senin, 15 Mei 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 16 Mei 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 17 Mei 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 18 Mei 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 19 Mei 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 20 Mei 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 21 Mei 2023</t>
+  </si>
+  <si>
+    <t>Senin, 22 Mei 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 23 Mei 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 24 Mei 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 25 Mei 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 26 Mei 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 27 Mei 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 28 Mei 2023</t>
+  </si>
+  <si>
+    <t>Senin, 29 Mei 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 30 Mei 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 31 Mei 2023</t>
+  </si>
+  <si>
+    <t>10:09:43</t>
   </si>
   <si>
     <t>Hadir</t>
   </si>
   <si>
-    <t>14,626 kilometer, TERLAMBAT 2 jam 29 menit</t>
-  </si>
-  <si>
-    <t>Sabtu, 13 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 14 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 15 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 16 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 17 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 18 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 19 Mei 2023</t>
-  </si>
-  <si>
-    <t>21:01:29</t>
-  </si>
-  <si>
-    <t>22:22:48</t>
-  </si>
-  <si>
-    <t>34,163 kilometer, TERLAMBAT 13 jam 47 menit</t>
-  </si>
-  <si>
-    <t>Sabtu, 20 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 21 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 22 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 23 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 24 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 25 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 26 Mei 2023</t>
-  </si>
-  <si>
-    <t>Sabtu, 27 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 28 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 29 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 30 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 31 Mei 2023</t>
+    <t>13,543 kilometer, TERLAMBAT 2 jam 55 menit</t>
   </si>
   <si>
     <t>Izin</t>
@@ -663,20 +654,14 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -685,7 +670,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -696,7 +681,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -705,7 +690,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -714,7 +699,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -723,7 +708,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -732,24 +717,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -758,7 +735,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -769,7 +746,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -778,7 +755,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -787,7 +764,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -796,7 +773,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -805,7 +782,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -814,7 +791,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -823,7 +800,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -834,7 +811,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -843,7 +820,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -852,24 +829,30 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -877,7 +860,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -885,10 +868,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B37" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Penyempurnaan dan perbaikan bug untuk halaman Admin CRUD Pengguna
</commit_message>
<xml_diff>
--- a/rekap_presensi.xlsx
+++ b/rekap_presensi.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>Tanggal</t>
   </si>
@@ -32,103 +32,106 @@
     <t>Keterangan</t>
   </si>
   <si>
-    <t>Senin, 1 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 2 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 3 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 4 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 5 Mei 2023</t>
-  </si>
-  <si>
-    <t>Sabtu, 6 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 7 Mei 2023</t>
+    <t>Kamis, 1 Juni 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 2 Juni 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 3 Juni 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 4 Juni 2023</t>
   </si>
   <si>
     <t>Libur Akhir Pekan</t>
   </si>
   <si>
-    <t>Senin, 8 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 9 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 10 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 11 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 12 Mei 2023</t>
-  </si>
-  <si>
-    <t>Sabtu, 13 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 14 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 15 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 16 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 17 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 18 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 19 Mei 2023</t>
-  </si>
-  <si>
-    <t>Sabtu, 20 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 21 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 22 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 23 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 24 Mei 2023</t>
-  </si>
-  <si>
-    <t>Kamis, 25 Mei 2023</t>
-  </si>
-  <si>
-    <t>Jumat, 26 Mei 2023</t>
-  </si>
-  <si>
-    <t>Sabtu, 27 Mei 2023</t>
-  </si>
-  <si>
-    <t>Minggu, 28 Mei 2023</t>
-  </si>
-  <si>
-    <t>Senin, 29 Mei 2023</t>
-  </si>
-  <si>
-    <t>Selasa, 30 Mei 2023</t>
-  </si>
-  <si>
-    <t>Rabu, 31 Mei 2023</t>
+    <t>Senin, 5 Juni 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 6 Juni 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 7 Juni 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 8 Juni 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 9 Juni 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 10 Juni 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 11 Juni 2023</t>
+  </si>
+  <si>
+    <t>Senin, 12 Juni 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 13 Juni 2023</t>
+  </si>
+  <si>
+    <t>12:41:13</t>
   </si>
   <si>
     <t>Hadir</t>
+  </si>
+  <si>
+    <t>13 kilometer, TERLAMBAT 4 jam 42 menit</t>
+  </si>
+  <si>
+    <t>Rabu, 14 Juni 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 15 Juni 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 16 Juni 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 17 Juni 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 18 Juni 2023</t>
+  </si>
+  <si>
+    <t>Senin, 19 Juni 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 20 Juni 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 21 Juni 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 22 Juni 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 23 Juni 2023</t>
+  </si>
+  <si>
+    <t>Sabtu, 24 Juni 2023</t>
+  </si>
+  <si>
+    <t>Minggu, 25 Juni 2023</t>
+  </si>
+  <si>
+    <t>Senin, 26 Juni 2023</t>
+  </si>
+  <si>
+    <t>Selasa, 27 Juni 2023</t>
+  </si>
+  <si>
+    <t>Rabu, 28 Juni 2023</t>
+  </si>
+  <si>
+    <t>Kamis, 29 Juni 2023</t>
+  </si>
+  <si>
+    <t>Jumat, 30 Juni 2023</t>
   </si>
   <si>
     <t>Izin</t>
@@ -511,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A34" sqref="A34:B37"/>
+      <selection activeCell="A33" sqref="A33:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -571,17 +574,19 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -590,7 +595,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -598,15 +603,13 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
@@ -636,13 +639,15 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
@@ -657,25 +662,29 @@
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -684,7 +693,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -693,7 +702,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -701,17 +710,19 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -720,7 +731,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -728,19 +739,17 @@
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -749,7 +758,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -758,7 +767,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -766,17 +775,19 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -785,7 +796,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -793,19 +804,17 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -814,25 +823,24 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -840,7 +848,7 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2">
         <v>0</v>
@@ -848,18 +856,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>